<commit_message>
Alta Materia/Curso v1 [2019-06-30 19:42 ]
 - Se corrigen las referencias de carga del formulario de "AltaMateria"
</commit_message>
<xml_diff>
--- a/devResource/DB-SistEduc-Valores.xlsx
+++ b/devResource/DB-SistEduc-Valores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josee\git\labv-tp-gestioneducativa-spring\devResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{C85BDE74-A87C-4F75-BDA0-96760FBE97FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{AD5962D4-4DC1-4051-9061-E4A5209476EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.TiposDe" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FB59840E-C63A-42EB-9976-A7EA5878B363}" diskRevisions="1" revisionId="62" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8B042417-937E-4B15-9FB2-BAFC9C7D2975}" diskRevisions="1" revisionId="67" version="5">
   <header guid="{8151FE72-FD84-4569-B050-C101B7C95C3F}" dateTime="2019-06-23T01:12:49" maxSheetId="5" userName="José Escobar" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -483,6 +483,14 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{8B042417-937E-4B15-9FB2-BAFC9C7D2975}" dateTime="2019-06-30T19:46:41" maxSheetId="5" userName="José Escobar" r:id="rId5" minRId="63" maxRId="67">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1232,8 +1240,65 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="63" sId="3">
+    <oc r="F1">
+      <f>CONCATENATE("INSERT into cursos SET idCurso=",A1,", nombreCurso='",B1,
+"', anio=",C1,", idPeriodo=",D1,", dniProfesor='",E1,"' ;")</f>
+    </oc>
+    <nc r="F1">
+      <f>CONCATENATE("INSERT into curso SET idCurso=",A1,", nombreCurso='",B1,
+"', anio=",C1,", idPeriodo=",D1,", dniProfesor='",E1,"' ;")</f>
+    </nc>
+  </rcc>
+  <rcc rId="64" sId="3">
+    <oc r="F2">
+      <f>CONCATENATE("INSERT into cursos SET idCurso=",A2,", nombreCurso='",B2,
+"', anio=",C2,", idPeriodo=",D2,", dniProfesor='",E2,"' ;")</f>
+    </oc>
+    <nc r="F2">
+      <f>CONCATENATE("INSERT into curso SET idCurso=",A2,", nombreCurso='",B2,
+"', anio=",C2,", idPeriodo=",D2,", dniProfesor='",E2,"' ;")</f>
+    </nc>
+  </rcc>
+  <rcc rId="65" sId="3">
+    <oc r="F3">
+      <f>CONCATENATE("INSERT into cursos SET idCurso=",A3,", nombreCurso='",B3,
+"', anio=",C3,", idPeriodo=",D3,", dniProfesor='",E3,"' ;")</f>
+    </oc>
+    <nc r="F3">
+      <f>CONCATENATE("INSERT into curso SET idCurso=",A3,", nombreCurso='",B3,
+"', anio=",C3,", idPeriodo=",D3,", dniProfesor='",E3,"' ;")</f>
+    </nc>
+  </rcc>
+  <rcc rId="66" sId="3">
+    <oc r="F4">
+      <f>CONCATENATE("INSERT into cursos SET idCurso=",A4,", nombreCurso='",B4,
+"', anio=",C4,", idPeriodo=",D4,", dniProfesor='",E4,"' ;")</f>
+    </oc>
+    <nc r="F4">
+      <f>CONCATENATE("INSERT into curso SET idCurso=",A4,", nombreCurso='",B4,
+"', anio=",C4,", idPeriodo=",D4,", dniProfesor='",E4,"' ;")</f>
+    </nc>
+  </rcc>
+  <rcc rId="67" sId="3">
+    <oc r="F5">
+      <f>CONCATENATE("INSERT into cursos SET idCurso=",A5,", nombreCurso='",B5,
+"', anio=",C5,", idPeriodo=",D5,", dniProfesor='",E5,"' ;")</f>
+    </oc>
+    <nc r="F5">
+      <f>CONCATENATE("INSERT into curso SET idCurso=",A5,", nombreCurso='",B5,
+"', anio=",C5,", idPeriodo=",D5,", dniProfesor='",E5,"' ;")</f>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{FB59840E-C63A-42EB-9976-A7EA5878B363}" name="José Escobar" id="-206723224" dateTime="2019-06-30T18:30:10"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1559,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1776,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,8 +2396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F2:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,9 +2427,9 @@
         <v>88</v>
       </c>
       <c r="F1" t="str">
-        <f t="shared" ref="F1:F4" si="0">CONCATENATE("INSERT into cursos SET idCurso=",A1,", nombreCurso='",B1,
+        <f>CONCATENATE("INSERT into curso SET idCurso=",A1,", nombreCurso='",B1,
 "', anio=",C1,", idPeriodo=",D1,", dniProfesor='",E1,"' ;")</f>
-        <v>INSERT into cursos SET idCurso=idCurso, nombreCurso='nombreCurso', anio=anio, idPeriodo=cuatrimestre, dniProfesor='dniProfesor' ;</v>
+        <v>INSERT into curso SET idCurso=idCurso, nombreCurso='nombreCurso', anio=anio, idPeriodo=cuatrimestre, dniProfesor='dniProfesor' ;</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2384,8 +2449,9 @@
         <v>60</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into cursos SET idCurso=1, nombreCurso='Programación', anio=2019, idPeriodo=1, dniProfesor='221' ;</v>
+        <f t="shared" ref="F2:F5" si="0">CONCATENATE("INSERT into curso SET idCurso=",A2,", nombreCurso='",B2,
+"', anio=",C2,", idPeriodo=",D2,", dniProfesor='",E2,"' ;")</f>
+        <v>INSERT into curso SET idCurso=1, nombreCurso='Programación', anio=2019, idPeriodo=1, dniProfesor='221' ;</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2406,7 +2472,7 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into cursos SET idCurso=2, nombreCurso='Matemáticas', anio=2019, idPeriodo=1, dniProfesor='222' ;</v>
+        <v>INSERT into curso SET idCurso=2, nombreCurso='Matemáticas', anio=2019, idPeriodo=1, dniProfesor='222' ;</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2427,7 +2493,7 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into cursos SET idCurso=3, nombreCurso='Inglés', anio=2019, idPeriodo=1, dniProfesor='223' ;</v>
+        <v>INSERT into curso SET idCurso=3, nombreCurso='Inglés', anio=2019, idPeriodo=1, dniProfesor='223' ;</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2447,9 +2513,8 @@
         <v>61</v>
       </c>
       <c r="F5" t="str">
-        <f>CONCATENATE("INSERT into cursos SET idCurso=",A5,", nombreCurso='",B5,
-"', anio=",C5,", idPeriodo=",D5,", dniProfesor='",E5,"' ;")</f>
-        <v>INSERT into cursos SET idCurso=4, nombreCurso='Inglés Avanzado', anio=2019, idPeriodo=2, dniProfesor='223' ;</v>
+        <f t="shared" si="0"/>
+        <v>INSERT into curso SET idCurso=4, nombreCurso='Inglés Avanzado', anio=2019, idPeriodo=2, dniProfesor='223' ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ABML de tipo de Examen [2019-07-16 05:29 josee]
 - Se prepara gestión ABML de Tipo de Examen
 - Diseño inicio admin

Signed-off-by: jescobar09 <joseescobar095@gmail.com>
</commit_message>
<xml_diff>
--- a/devResource/DB-SistEduc-Valores.xlsx
+++ b/devResource/DB-SistEduc-Valores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josee\git\labv-tp-gestioneducativa-spring\devResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{AD5962D4-4DC1-4051-9061-E4A5209476EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3A93E7C9-7FCE-46BF-B1A6-3C78AE51B68C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.TiposDe" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="107">
   <si>
     <t xml:space="preserve"> nombre</t>
   </si>
@@ -261,12 +261,6 @@
     <t>frgp3</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>C. Alumno</t>
-  </si>
-  <si>
     <t>3333333333</t>
   </si>
   <si>
@@ -325,6 +319,42 @@
   </si>
   <si>
     <t>000</t>
+  </si>
+  <si>
+    <t>Ayelén</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>Malloti</t>
+  </si>
+  <si>
+    <t>Silvia</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>De Satigny</t>
+  </si>
+  <si>
+    <t>Tercero García</t>
+  </si>
+  <si>
+    <t>Trueba</t>
+  </si>
+  <si>
+    <t>Del Valle</t>
   </si>
 </sst>
 </file>
@@ -450,7 +480,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8B042417-937E-4B15-9FB2-BAFC9C7D2975}" diskRevisions="1" revisionId="67" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4E21A7F2-BFA8-47CB-9CCD-D474D96D9B53}" diskRevisions="1" revisionId="81" version="7">
   <header guid="{8151FE72-FD84-4569-B050-C101B7C95C3F}" dateTime="2019-06-23T01:12:49" maxSheetId="5" userName="José Escobar" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -491,6 +521,22 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{30F99AAB-41C0-4870-B1B2-8B4ACFA83E0C}" dateTime="2019-07-16T05:21:03" maxSheetId="5" userName="José Escobar" r:id="rId6" minRId="68" maxRId="79">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4E21A7F2-BFA8-47CB-9CCD-D474D96D9B53}" dateTime="2019-07-16T05:21:30" maxSheetId="5" userName="José Escobar" r:id="rId7" minRId="80" maxRId="81">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1295,7 +1341,229 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="2" xfDxf="1" sqref="B7" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" xfDxf="1" sqref="C7" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" xfDxf="1" sqref="C7" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" xfDxf="1" sqref="B7" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="68" sId="2" xfDxf="1" dxf="1">
+    <oc r="B9" t="inlineStr">
+      <is>
+        <t>Juan</t>
+      </is>
+    </oc>
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>Clara</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="69" sId="2" xfDxf="1" dxf="1">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>Juan</t>
+      </is>
+    </oc>
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>Alba</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="70" sId="2" xfDxf="1" dxf="1">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>Juan</t>
+      </is>
+    </oc>
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>Pedro</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="71" sId="2" xfDxf="1" dxf="1">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>Juan</t>
+      </is>
+    </oc>
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>Jaime</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="72" sId="2" xfDxf="1" dxf="1">
+    <oc r="C11" t="inlineStr">
+      <is>
+        <t>C. Alumno</t>
+      </is>
+    </oc>
+    <nc r="C11" t="inlineStr">
+      <is>
+        <t>De Satigny</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="73" sId="2" xfDxf="1" dxf="1">
+    <oc r="C12" t="inlineStr">
+      <is>
+        <t>C. Alumno</t>
+      </is>
+    </oc>
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>Tercero García</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="74" sId="2">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>Tamara</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>Silvia</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="75" sId="2">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>A. Profe</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Malloti</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="76" sId="2">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>Tamara</t>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>Blanca</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="77" sId="2">
+    <oc r="C7" t="inlineStr">
+      <is>
+        <t>A. Profe</t>
+      </is>
+    </oc>
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Trueba</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="78" sId="2">
+    <oc r="C10" t="inlineStr">
+      <is>
+        <t>C. Alumno</t>
+      </is>
+    </oc>
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Trueba</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="79" sId="2">
+    <oc r="C9" t="inlineStr">
+      <is>
+        <t>C. Alumno</t>
+      </is>
+    </oc>
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Del Valle</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="80" sId="2" xfDxf="1" dxf="1">
+    <oc r="C7" t="inlineStr">
+      <is>
+        <t>Trueba</t>
+      </is>
+    </oc>
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Flores</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="81" sId="2" xfDxf="1" dxf="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>Blanca</t>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>Ayelén</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{FB59840E-C63A-42EB-9976-A7EA5878B363}" name="José Escobar" id="-206723224" dateTime="2019-06-30T18:30:10"/>
 </users>
@@ -1624,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +2087,7 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="2"/>
@@ -1841,8 +2109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,10 +2144,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1912,31 +2180,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>19</v>
@@ -1957,22 +2225,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
@@ -2000,22 +2268,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
@@ -2043,22 +2311,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>14</v>
@@ -2095,7 +2363,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
@@ -2128,16 +2396,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
@@ -2162,7 +2430,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into usuario SET idUsuario=6, nombre='Tamara', apellido='A. Profe', dni='222', calleNombre='calle profe ', calleAltura='222', fechaNac=STR_TO_DATE('01/01/2000','%d/%m/%Y') , nroTelefono='22222', mail='profe@gmail.com2', clave='utn123', idTipoUsuario=2, habilitado=1 ;</v>
+        <v>INSERT into usuario SET idUsuario=6, nombre='Ayelén', apellido='Flores', dni='222', calleNombre='calle profe ', calleAltura='222', fechaNac=STR_TO_DATE('01/01/2000','%d/%m/%Y') , nroTelefono='22222', mail='profe@gmail.com2', clave='utn123', idTipoUsuario=2, habilitado=1 ;</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2170,16 +2438,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -2204,7 +2472,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into usuario SET idUsuario=7, nombre='Tamara', apellido='A. Profe', dni='223', calleNombre='calle profe ', calleAltura='222', fechaNac=STR_TO_DATE('01/01/2000','%d/%m/%Y') , nroTelefono='22222', mail='profe@gmail.com3', clave='utn123', idTipoUsuario=2, habilitado=1 ;</v>
+        <v>INSERT into usuario SET idUsuario=7, nombre='Silvia', apellido='Malloti', dni='223', calleNombre='calle profe ', calleAltura='222', fechaNac=STR_TO_DATE('01/01/2000','%d/%m/%Y') , nroTelefono='22222', mail='profe@gmail.com3', clave='utn123', idTipoUsuario=2, habilitado=1 ;</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2212,19 +2480,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>11</v>
@@ -2246,7 +2514,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into usuario SET idUsuario=8, nombre='Juan', apellido='C. Alumno', dni='11111', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com1', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
+        <v>INSERT into usuario SET idUsuario=8, nombre='Clara', apellido='Del Valle', dni='11111', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com1', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2254,19 +2522,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>11</v>
@@ -2288,7 +2556,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into usuario SET idUsuario=9, nombre='Juan', apellido='C. Alumno', dni='11112', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com2', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
+        <v>INSERT into usuario SET idUsuario=9, nombre='Jaime', apellido='Trueba', dni='11112', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com2', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2296,19 +2564,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
@@ -2330,7 +2598,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into usuario SET idUsuario=10, nombre='Juan', apellido='C. Alumno', dni='11113', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com3', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
+        <v>INSERT into usuario SET idUsuario=10, nombre='Alba', apellido='De Satigny', dni='11113', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com3', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2338,19 +2606,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
@@ -2372,7 +2640,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into usuario SET idUsuario=11, nombre='Juan', apellido='C. Alumno', dni='11114', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com4', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
+        <v>INSERT into usuario SET idUsuario=11, nombre='Pedro', apellido='Tercero García', dni='11114', calleNombre='calle alumno', calleAltura='111', fechaNac=STR_TO_DATE('01/12/2000','%d/%m/%Y') , nroTelefono='11111', mail='alumno@gmail.com4', clave='utn123', idTipoUsuario=1, habilitado=1 ;</v>
       </c>
     </row>
   </sheetData>
@@ -2396,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,7 +2692,7 @@
         <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F1" t="str">
         <f>CONCATENATE("INSERT into curso SET idCurso=",A1,", nombreCurso='",B1,

</xml_diff>